<commit_message>
V1 opt by pulp
</commit_message>
<xml_diff>
--- a/data/零件需求.XLSX
+++ b/data/零件需求.XLSX
@@ -48,7 +48,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -63,6 +63,18 @@
       <sz val="9"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -88,8 +100,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -105,8 +119,10 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -408,7 +424,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>